<commit_message>
Izzy updated scripts and data
</commit_message>
<xml_diff>
--- a/data/test_accuracy_error.xlsx
+++ b/data/test_accuracy_error.xlsx
@@ -8,14 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/izzyrich/Documents/Edinburgh Year 4/dissertation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0633B199-49F1-BB42-AF42-4850C4D62323}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5EF5016-2F24-F346-A1CC-827AA817171E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="460" windowWidth="27320" windowHeight="14900" xr2:uid="{76A2E617-E315-7846-B2E7-6D902E1B1D35}"/>
+    <workbookView xWindow="1420" yWindow="-21140" windowWidth="27320" windowHeight="14900" activeTab="1" xr2:uid="{76A2E617-E315-7846-B2E7-6D902E1B1D35}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="no_cloud_corect" sheetId="1" r:id="rId1"/>
+    <sheet name="cloud_correct" sheetId="3" r:id="rId2"/>
+    <sheet name="overall_cloud_correct" sheetId="2" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">no_cloud_corect!$A$1:$C$28</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="59">
   <si>
     <t>year</t>
   </si>
@@ -124,9 +128,6 @@
     <t>RF_error_matrix</t>
   </si>
   <si>
-    <t>[[92508,0,0,584,2,1,0],[365,4017,0,200,5,1,0],[70,0,771,66,0,0,0],[1188,2,0,51649,2,0,0],[614,0,0,247,5875,0,0],[466,0,0,94,3,3351,0],[215,0,0,190,5,0,2348]]</t>
-  </si>
-  <si>
     <t>[[19608, 39, 0, 3452, 130, 26, 5], [584, 0, 0, 489, 1, 1, 0], [266, 2, 0, 185, 1, 0, 0], [5660, 15, 1, 7408, 22, 5, 7], [1370, 2, 0, 225, 171, 0, 14], [881, 0, 0, 242, 5, 0, 0], [439, 1, 0, 322, 0, 0, 0]]</t>
   </si>
   <si>
@@ -140,6 +141,78 @@
   </si>
   <si>
     <t>[[19280, 17, 0, 3878, 44, 32, 9], [567, 0, 0, 508, 0, 0, 0], [169, 1, 0, 283, 0, 1, 0], [4036, 12, 8, 8990, 49, 11, 12], [1169, 2, 0, 325, 281, 2, 3], [845, 3, 0, 278, 0, 2, 0], [379, 0, 0, 337, 26, 0, 20]]</t>
+  </si>
+  <si>
+    <t>[[92261,0,0,745,17,2,0],[402,3951,0,226,7,2,0],[37,0,776,93,1,0,0],[1358,2,0,51475,6,0,0],[618,0,0,324,5790,1,3],[551,0,0,115,7,3240,0],[206,0,0,255,20,0,2277]]</t>
+  </si>
+  <si>
+    <t>[[19688, 8, 1, 3459, 61, 27, 8], [548, 0, 0, 526, 1, 0, 0], [141, 0, 0, 312, 1, 0, 0], [2997, 12, 1, 9986, 41, 6, 41], [1063, 2, 0, 372, 344, 1, 0], [862, 0, 0, 252, 6, 8, 0], [280, 0, 0, 439, 33, 0, 10]]</t>
+  </si>
+  <si>
+    <t>[[18496, 4, 0, 4621, 117, 11, 11], [363, 0, 0, 710, 2, 0, 0], [69, 0, 0, 384, 1, 0, 0], [2510, 17, 0, 10502, 46, 26, 17], [873, 2, 0, 583, 317, 1, 6], [849, 0, 0, 266, 12, 1, 0], [375, 2, 0, 360, 14, 0, 11]]</t>
+  </si>
+  <si>
+    <t>[[18322, 3, 0, 4506, 342, 24, 8], [376, 2, 0, 691, 0, 2, 4], [49, 0, 0, 404, 0, 0, 1], [2689, 14, 0, 10202, 74, 24, 25], [937, 1, 0, 526, 318, 0, 0], [792, 0, 0, 317, 15, 4, 0], [302, 0, 0, 443, 8, 0, 9]]</t>
+  </si>
+  <si>
+    <t>[[17314, 7, 0, 5708, 172, 32, 27], [302, 0, 0, 768, 2, 0, 3], [40, 0, 0, 402, 1, 0, 11], [1725, 12, 0, 11322, 25, 0, 34], [785, 11, 0, 666, 310, 2, 8], [736, 0, 0, 379, 4, 4, 5], [255, 0, 0, 484, 16, 0, 7]]</t>
+  </si>
+  <si>
+    <t>[[18780, 2, 0, 4387, 71, 15, 5], [424, 0, 0, 651, 0, 0, 0], [68, 0, 0, 383, 0, 0, 3], [2228, 0, 0, 10836, 25, 19, 10], [946, 2, 2, 526, 291, 9, 6], [856, 0, 0, 264, 7, 1, 0], [303, 0, 2, 437, 15, 0, 5]]</t>
+  </si>
+  <si>
+    <t>[[19416, 2, 0, 3599, 127, 36, 3], [449, 2, 0, 624, 0, 0, 0], [112, 0, 0, 325, 5, 5, 7], [3212, 4, 2, 9844, 26, 17, 9], [1010, 0, 0, 440, 317, 2, 13], [916, 0, 0, 199, 13, 0, 0], [319, 0, 0, 397, 41, 0, 5]]</t>
+  </si>
+  <si>
+    <t>[[19880, 2, 0, 3317, 35, 26, 0], [604, 0, 0, 471, 0, 0, 0], [124, 0, 0, 328, 0, 0, 2], [3821, 6, 1, 9242, 40, 6, 2], [1071, 0, 0, 353, 347, 4, 7], [920, 0, 0, 191, 9, 8, 0], [336, 0, 0, 414, 4, 2, 6]]</t>
+  </si>
+  <si>
+    <t>[[19478, 7, 0, 3222, 192, 25, 11], [551, 2, 0, 513, 0, 0, 0], [155, 0, 0, 268, 14, 0, 3], [4106, 6, 1, 8650, 114, 12, 4], [1098, 0, 0, 324, 314, 1, 5], [901, 0, 0, 168, 29, 1, 0], [346, 0, 0, 347, 15, 0, 9]]</t>
+  </si>
+  <si>
+    <t>[[18143, 7, 0, 3686, 178, 44, 33], [523, 0, 0, 484, 20, 1, 2], [114, 0, 0, 332, 1, 0, 0], [4347, 7, 0, 7821, 115, 56, 41], [911, 2, 0, 341, 291, 0, 5], [819, 0, 0, 202, 13, 2, 0], [294, 0, 0, 432, 26, 0, 10]]</t>
+  </si>
+  <si>
+    <t>[[19827, 9, 0, 3228, 108, 44, 2], [635, 2, 0, 436, 0, 2, 0], [142, 0, 0, 311, 0, 0, 1], [4498, 6, 0, 8522, 32, 33, 6], [1035, 3, 0, 442, 296, 2, 4], [915, 0, 0, 203, 6, 4, 0], [312, 0, 0, 411, 27, 0, 12]]</t>
+  </si>
+  <si>
+    <t>[[20214, 3, 0, 2850, 38, 16, 6], [604, 0, 0, 471, 0, 0, 0], [121, 0, 0, 333, 0, 0, 0], [4260, 4, 0, 8665, 72, 63, 4], [1139, 4, 0, 321, 316, 0, 2], [937, 0, 0, 188, 2, 1, 0], [341, 0, 0, 384, 20, 0, 17]]</t>
+  </si>
+  <si>
+    <t>[[18909, 8, 0, 3641, 77, 33, 3], [487, 0, 0, 536, 0, 0, 0], [137, 0, 0, 316, 1, 0, 0], [3593, 4, 0, 8944, 57, 74, 21], [1113, 2, 0, 327, 333, 2, 5], [899, 0, 0, 160, 8, 2, 0], [291, 0, 0, 394, 32, 0, 14]]</t>
+  </si>
+  <si>
+    <t>[[16860, 7, 0, 4474, 269, 24, 13], [386, 3, 0, 581, 6, 0, 17], [79, 0, 0, 375, 0, 0, 0], [2643, 12, 0, 9650, 155, 17, 22], [896, 2, 1, 518, 302, 0, 4], [706, 0, 0, 312, 13, 2, 0], [290, 3, 0, 434, 26, 2, 7]]</t>
+  </si>
+  <si>
+    <t>[[20738, 5, 0, 2454, 43, 18, 2], [663, 2, 0, 403, 0, 5, 2], [157, 0, 0, 294, 2, 0, 1], [4826, 4, 0, 8170, 37, 79, 2], [1115, 1, 2, 339, 319, 2, 4], [982, 0, 0, 142, 3, 0, 1], [409, 0, 0, 344, 7, 0, 2]]</t>
+  </si>
+  <si>
+    <t>[[19396, 6, 2, 3723, 93, 23, 9], [515, 0, 0, 560, 0, 0, 0], [104, 0, 0, 337, 7, 0, 6], [2634, 3, 0, 10443, 27, 4, 7], [968, 2, 0, 463, 344, 3, 2], [848, 0, 0, 262, 15, 3, 0], [301, 0, 0, 426, 22, 0, 13]]</t>
+  </si>
+  <si>
+    <t>[[17430, 10, 0, 3136, 429, 22, 13], [525, 0, 0, 506, 4, 4, 0], [115, 2, 0, 298, 2, 0, 0], [3546, 11, 0, 8372, 101, 42, 2], [863, 3, 0, 420, 363, 0, 4], [816, 2, 0, 199, 7, 2, 0], [228, 2, 0, 465, 31, 0, 8]]</t>
+  </si>
+  <si>
+    <t>[[18425, 8, 0, 3129, 229, 24, 4], [495, 1, 0, 488, 0, 2, 0], [156, 0, 0, 257, 1, 0, 11], [3550, 4, 0, 8629, 74, 22, 20], [933, 2, 0, 335, 402, 1, 4], [800, 0, 0, 226, 13, 0, 2], [328, 0, 0, 339, 25, 0, 4]]</t>
+  </si>
+  <si>
+    <t>[[9880, 6, 0, 1815, 160, 14, 15], [100, 0, 0, 64, 0, 0, 0], [59, 2, 0, 251, 1, 0, 0], [1796, 8, 0, 4545, 23, 0, 6], [468, 2, 0, 247, 176, 2, 0], [474, 0, 0, 143, 0, 1, 0], [286, 0, 0, 159, 21, 1, 11]]</t>
+  </si>
+  <si>
+    <t>[[18834, 3, 0, 3129, 181, 11, 12], [563, 0, 0, 433, 21, 6, 0], [109, 0, 0, 291, 15, 2, 4], [4680, 19, 0, 6799, 229, 71, 29], [1018, 3, 0, 414, 286, 2, 8], [879, 0, 0, 182, 4, 4, 0], [320, 4, 0, 344, 33, 0, 3]]</t>
+  </si>
+  <si>
+    <t>[[19359, 10, 0, 3809, 33, 45, 4], [544, 0, 0, 531, 0, 0, 0], [95, 0, 0, 357, 1, 0, 1], [3526, 12, 0, 9543, 24, 5, 8], [1045, 7, 0, 417, 310, 0, 3], [897, 1, 0, 218, 7, 5, 0], [299, 2, 0, 425, 24, 4, 8]]</t>
+  </si>
+  <si>
+    <t>[[19792, 14, 0, 3216, 39, 52, 1], [546, 0, 0, 529, 0, 0, 0], [126, 0, 0, 324, 3, 0, 1], [5044, 2, 2, 7862, 37, 73, 10], [1161, 0, 0, 324, 263, 1, 0], [921, 0, 0, 206, 0, 1, 0], [373, 0, 0, 374, 8, 2, 5]]</t>
+  </si>
+  <si>
+    <t>[[18993, 11, 0, 4056, 93, 13, 10], [541, 2, 0, 531, 0, 0, 1], [156, 0, 0, 297, 1, 0, 0], [3920, 13, 0, 9096, 31, 44, 10], [1072, 2, 0, 352, 313, 1, 1], [844, 0, 0, 275, 8, 1, 0], [371, 0, 0, 346, 21, 1, 15]]</t>
+  </si>
+  <si>
+    <t>[[18477, 11, 0, 4407, 246, 30, 32], [435, 0, 0, 615, 4, 6, 12], [60, 0, 0, 391, 1, 0, 2], [3173, 6, 2, 9578, 142, 32, 57], [875, 0, 0, 561, 288, 7, 10], [805, 0, 0, 298, 5, 3, 0], [296, 0, 0, 445, 20, 0, 1]]</t>
   </si>
 </sst>
 </file>
@@ -147,7 +220,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.000000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -181,7 +254,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,10 +569,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00FB4CC6-6F0E-7440-803D-858E8BFE0C52}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -519,7 +593,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1985</v>
       </c>
@@ -541,7 +615,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1987</v>
       </c>
@@ -552,7 +626,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1988</v>
       </c>
@@ -574,7 +648,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1990</v>
       </c>
@@ -607,7 +681,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1993</v>
       </c>
@@ -662,7 +736,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1998</v>
       </c>
@@ -684,7 +758,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2000</v>
       </c>
@@ -706,7 +780,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2002</v>
       </c>
@@ -717,7 +791,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2003</v>
       </c>
@@ -728,7 +802,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2004</v>
       </c>
@@ -772,7 +846,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2008</v>
       </c>
@@ -802,7 +876,7 @@
         <v>0.65386372928641801</v>
       </c>
       <c r="C27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -813,12 +887,12 @@
         <v>0.68719786429999996</v>
       </c>
       <c r="C28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B38">
         <f>AVERAGE(B2:B28)</f>
@@ -827,7 +901,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B39">
         <f>MAX(B2:B28)</f>
@@ -836,11 +910,343 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B40">
         <f>MIN(B2:B28)</f>
         <v>0.57897015320233702</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:C28" xr:uid="{9444BE47-4DD2-EA48-BE8C-0576034B5379}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="0.650328291"/>
+        <filter val="0.653166262"/>
+        <filter val="0.653863729"/>
+        <filter val="0.658505496"/>
+        <filter val="0.664397893"/>
+        <filter val="0.665239664"/>
+        <filter val="0.675701676"/>
+        <filter val="0.679164963"/>
+        <filter val="0.682002934"/>
+        <filter val="0.687197864"/>
+        <filter val="0.687414320"/>
+        <filter val="0.687919382"/>
+        <filter val="0.691671276"/>
+        <filter val="0.698718103"/>
+        <filter val="0.700257341"/>
+        <filter val="0.701099113"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D3BCE67-7F25-AA4D-A56D-CAF87EAC7D06}">
+  <dimension ref="A1:C33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="156.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1989</v>
+      </c>
+      <c r="B2">
+        <v>0.70533201860000005</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1990</v>
+      </c>
+      <c r="B3">
+        <v>0.68582004689999998</v>
+      </c>
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1991</v>
+      </c>
+      <c r="B4">
+        <v>0.69645701599999998</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1992</v>
+      </c>
+      <c r="B5">
+        <v>0.69643329570000001</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1993</v>
+      </c>
+      <c r="B6">
+        <v>0.68584285749999996</v>
+      </c>
+      <c r="C6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1994</v>
+      </c>
+      <c r="B7">
+        <v>0.71942567160000004</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1995</v>
+      </c>
+      <c r="B8">
+        <v>0.70302316070000004</v>
+      </c>
+      <c r="C8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1996</v>
+      </c>
+      <c r="B9">
+        <v>0.71290182660000001</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1997</v>
+      </c>
+      <c r="B10">
+        <v>0.72644391519999996</v>
+      </c>
+      <c r="C10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1998</v>
+      </c>
+      <c r="B11">
+        <v>0.68912408179999995</v>
+      </c>
+      <c r="C11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1999</v>
+      </c>
+      <c r="B12">
+        <v>0.70908391260000003</v>
+      </c>
+      <c r="C12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2000</v>
+      </c>
+      <c r="B13">
+        <v>0.70515882190000001</v>
+      </c>
+      <c r="C13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2001</v>
+      </c>
+      <c r="B14">
+        <v>0.6958329258</v>
+      </c>
+      <c r="C14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2002</v>
+      </c>
+      <c r="B15">
+        <v>0.70471643520000005</v>
+      </c>
+      <c r="C15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>2003</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.66570804979999998</v>
+      </c>
+      <c r="C16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>2004</v>
+      </c>
+      <c r="B17">
+        <v>0.66832048440000003</v>
+      </c>
+      <c r="C17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>2005</v>
+      </c>
+      <c r="B18">
+        <v>0.69040851719999996</v>
+      </c>
+      <c r="C18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>2006</v>
+      </c>
+      <c r="B19">
+        <v>0.6958329258</v>
+      </c>
+      <c r="C19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>2007</v>
+      </c>
+      <c r="B20">
+        <v>0.70569620249999998</v>
+      </c>
+      <c r="C20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>2008</v>
+      </c>
+      <c r="B21">
+        <v>0.67590530599999998</v>
+      </c>
+      <c r="C21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>2009</v>
+      </c>
+      <c r="B22">
+        <v>0.69767211740000001</v>
+      </c>
+      <c r="C22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>2010</v>
+      </c>
+      <c r="B23">
+        <v>0.68577771340000004</v>
+      </c>
+      <c r="C23" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>2011</v>
+      </c>
+      <c r="B24">
+        <v>0.72311433179999995</v>
+      </c>
+      <c r="C24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31">
+        <f>AVERAGE(B2:B24)</f>
+        <v>0.6975665928</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32">
+        <f>MIN(B2:B24)</f>
+        <v>0.66570804979999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <f>MAX(B2:B24)</f>
+        <v>0.72644391519999996</v>
       </c>
     </row>
   </sheetData>
@@ -848,12 +1254,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2E1821D-B1B8-DB4E-89D6-075BD4470CC9}">
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -871,10 +1277,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>0.97379260975861204</v>
+        <v>9696664400854530</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Izzy prepared for meeting with Isla
</commit_message>
<xml_diff>
--- a/data/test_accuracy_error.xlsx
+++ b/data/test_accuracy_error.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/izzyrich/Documents/Edinburgh Year 4/dissertation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5EF5016-2F24-F346-A1CC-827AA817171E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B1ABAA-9422-244A-8C62-1FDE91326371}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="-21140" windowWidth="27320" windowHeight="14900" activeTab="1" xr2:uid="{76A2E617-E315-7846-B2E7-6D902E1B1D35}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="14900" activeTab="1" xr2:uid="{76A2E617-E315-7846-B2E7-6D902E1B1D35}"/>
   </bookViews>
   <sheets>
     <sheet name="no_cloud_corect" sheetId="1" r:id="rId1"/>
@@ -569,11 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00FB4CC6-6F0E-7440-803D-858E8BFE0C52}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -593,7 +592,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1985</v>
       </c>
@@ -615,7 +614,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1987</v>
       </c>
@@ -626,7 +625,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1988</v>
       </c>
@@ -648,7 +647,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1990</v>
       </c>
@@ -681,7 +680,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1993</v>
       </c>
@@ -736,7 +735,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1998</v>
       </c>
@@ -758,7 +757,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2000</v>
       </c>
@@ -780,7 +779,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2002</v>
       </c>
@@ -791,7 +790,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2003</v>
       </c>
@@ -802,7 +801,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2004</v>
       </c>
@@ -846,7 +845,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2008</v>
       </c>
@@ -918,28 +917,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C28" xr:uid="{9444BE47-4DD2-EA48-BE8C-0576034B5379}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="0.650328291"/>
-        <filter val="0.653166262"/>
-        <filter val="0.653863729"/>
-        <filter val="0.658505496"/>
-        <filter val="0.664397893"/>
-        <filter val="0.665239664"/>
-        <filter val="0.675701676"/>
-        <filter val="0.679164963"/>
-        <filter val="0.682002934"/>
-        <filter val="0.687197864"/>
-        <filter val="0.687414320"/>
-        <filter val="0.687919382"/>
-        <filter val="0.691671276"/>
-        <filter val="0.698718103"/>
-        <filter val="0.700257341"/>
-        <filter val="0.701099113"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:C28" xr:uid="{9444BE47-4DD2-EA48-BE8C-0576034B5379}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -949,7 +927,7 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>